<commit_message>
refactoring and error handling
</commit_message>
<xml_diff>
--- a/resources/ShowExcel.xlsx
+++ b/resources/ShowExcel.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="186">
   <si>
     <t>Apellidos</t>
   </si>
@@ -569,7 +569,13 @@
     <t>AC</t>
   </si>
   <si>
-    <t>papapappa</t>
+    <t>dfgh</t>
+  </si>
+  <si>
+    <t>P2222</t>
+  </si>
+  <si>
+    <t>Pr234</t>
   </si>
 </sst>
 </file>
@@ -1766,11 +1772,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="6" max="8" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="33" width="25.28515625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="33" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1784,7 +1790,7 @@
         <v>183</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>167</v>
@@ -1810,10 +1816,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="38" t="n">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="D2" s="38" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" s="38" t="n">
         <v>30.0</v>
@@ -1839,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>126</v>
@@ -2928,11 +2934,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="3" max="10" customWidth="true" style="11" width="4.85546875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="8" width="55.42578125" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="10" customWidth="true" style="11" width="4.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="8" width="55.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4269,11 +4275,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="3" max="14" customWidth="true" style="11" width="4.85546875" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" style="8" width="38.140625" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="14" customWidth="true" style="11" width="4.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="8" width="38.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6035,11 +6041,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="3" max="8" customWidth="true" style="11" width="4.85546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="8" width="48.7109375" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="8" customWidth="true" style="11" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="8" width="48.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7179,11 +7185,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="3" max="15" customWidth="true" style="11" width="4.85546875" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" style="8" width="45.42578125" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="15" customWidth="true" style="11" width="4.85546875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="8" width="45.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="6.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
refactoring, error handling, nota final javascript
</commit_message>
<xml_diff>
--- a/resources/ShowExcel.xlsx
+++ b/resources/ShowExcel.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="188">
   <si>
     <t>Apellidos</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>Pr234</t>
+  </si>
+  <si>
+    <t>dfghh</t>
+  </si>
+  <si>
+    <t>dfghhs</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>185</v>

</xml_diff>

<commit_message>
styles, fixed bugs, removed script
</commit_message>
<xml_diff>
--- a/resources/ShowExcel.xlsx
+++ b/resources/ShowExcel.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="197">
   <si>
     <t>Apellidos</t>
   </si>
@@ -582,6 +582,33 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>exercise2</t>
+  </si>
+  <si>
+    <t>ex2</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ejercicio1</t>
+  </si>
+  <si>
+    <t>ej1</t>
+  </si>
+  <si>
+    <t>ejercicio2</t>
+  </si>
+  <si>
+    <t>ej2</t>
+  </si>
+  <si>
+    <t>ejercicio3</t>
+  </si>
+  <si>
+    <t>ej3</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1794,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
@@ -1778,11 +1805,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="10.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="10.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="10.0" collapsed="true"/>
@@ -1806,7 +1833,13 @@
         <v>148</v>
       </c>
       <c r="F1" t="s">
-        <v>186</v>
+        <v>191</v>
+      </c>
+      <c r="G1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1826,7 +1859,13 @@
         <v>0.0</v>
       </c>
       <c r="F2" t="n">
-        <v>60.0</v>
+        <v>20.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1846,7 +1885,13 @@
         <v>148</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1868,6 +1913,12 @@
       <c r="F4" t="n">
         <v>0.0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -1888,6 +1939,12 @@
       <c r="F5" t="n">
         <v>0.0</v>
       </c>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
@@ -1908,6 +1965,12 @@
       <c r="F6" t="n">
         <v>0.0</v>
       </c>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -1928,6 +1991,12 @@
       <c r="F7" t="n">
         <v>0.0</v>
       </c>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
@@ -1948,6 +2017,12 @@
       <c r="F8" t="n">
         <v>0.0</v>
       </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
@@ -1968,6 +2043,12 @@
       <c r="F9" t="n">
         <v>0.0</v>
       </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -1988,6 +2069,12 @@
       <c r="F10" t="n">
         <v>0.0</v>
       </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
@@ -2008,6 +2095,12 @@
       <c r="F11" t="n">
         <v>0.0</v>
       </c>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
@@ -2028,6 +2121,12 @@
       <c r="F12" t="n">
         <v>0.0</v>
       </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
@@ -2048,6 +2147,12 @@
       <c r="F13" t="n">
         <v>0.0</v>
       </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
@@ -2068,6 +2173,12 @@
       <c r="F14" t="n">
         <v>0.0</v>
       </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
@@ -2088,6 +2199,12 @@
       <c r="F15" t="n">
         <v>0.0</v>
       </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
@@ -2108,6 +2225,12 @@
       <c r="F16" t="n">
         <v>0.0</v>
       </c>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
@@ -2128,6 +2251,12 @@
       <c r="F17" t="n">
         <v>0.0</v>
       </c>
+      <c r="G17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
@@ -2148,6 +2277,12 @@
       <c r="F18" t="n">
         <v>0.0</v>
       </c>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
@@ -2168,6 +2303,12 @@
       <c r="F19" t="n">
         <v>0.0</v>
       </c>
+      <c r="G19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
@@ -2188,6 +2329,12 @@
       <c r="F20" t="n">
         <v>0.0</v>
       </c>
+      <c r="G20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
@@ -2208,6 +2355,12 @@
       <c r="F21" t="n">
         <v>0.0</v>
       </c>
+      <c r="G21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
@@ -2228,6 +2381,12 @@
       <c r="F22" t="n">
         <v>0.0</v>
       </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
@@ -2248,6 +2407,12 @@
       <c r="F23" t="n">
         <v>0.0</v>
       </c>
+      <c r="G23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
@@ -2268,6 +2433,12 @@
       <c r="F24" t="n">
         <v>0.0</v>
       </c>
+      <c r="G24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
@@ -2288,6 +2459,12 @@
       <c r="F25" t="n">
         <v>0.0</v>
       </c>
+      <c r="G25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
@@ -2308,6 +2485,12 @@
       <c r="F26" t="n">
         <v>0.0</v>
       </c>
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
@@ -2328,6 +2511,12 @@
       <c r="F27" t="n">
         <v>0.0</v>
       </c>
+      <c r="G27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
@@ -2348,6 +2537,12 @@
       <c r="F28" t="n">
         <v>0.0</v>
       </c>
+      <c r="G28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
@@ -2368,6 +2563,12 @@
       <c r="F29" t="n">
         <v>0.0</v>
       </c>
+      <c r="G29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
@@ -2388,6 +2589,12 @@
       <c r="F30" t="n">
         <v>0.0</v>
       </c>
+      <c r="G30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
@@ -2408,6 +2615,12 @@
       <c r="F31" t="n">
         <v>0.0</v>
       </c>
+      <c r="G31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
@@ -2428,6 +2641,12 @@
       <c r="F32" t="n">
         <v>0.0</v>
       </c>
+      <c r="G32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
@@ -2448,6 +2667,12 @@
       <c r="F33" t="n">
         <v>0.0</v>
       </c>
+      <c r="G33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -2458,6 +2683,12 @@
       </c>
       <c r="D34" s="0"/>
       <c r="F34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H34" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>